<commit_message>
Modifier les fichiers de dé/connexion l'ajout d'animaux le profil
Modif sur les maquettes et le planning
Ajout du fichier phptohtml
</commit_message>
<xml_diff>
--- a/planning.xlsx
+++ b/planning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
   <si>
     <t>Planning réel du TPI</t>
   </si>
@@ -67,6 +67,24 @@
   </si>
   <si>
     <t>Créer le projet dans NetBeans et créer les pages</t>
+  </si>
+  <si>
+    <t>Faire l'inscription</t>
+  </si>
+  <si>
+    <t>Faire la dé/connexion</t>
+  </si>
+  <si>
+    <t>Faire la page profil</t>
+  </si>
+  <si>
+    <t>Faire les liens de l'index</t>
+  </si>
+  <si>
+    <t>Ajouter le bootstrap sur les pages déjà créées</t>
+  </si>
+  <si>
+    <t>Créer le fichier phptohtml</t>
   </si>
 </sst>
 </file>
@@ -410,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U17"/>
+  <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,11 +660,60 @@
         <v>4.5138888888888888E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="D17" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" s="2">
+        <v>6.9444444444444441E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2">
+        <v>7.6388888888888895E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="2">
         <v>2.0833333333333332E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
avancé la doc petites modif sur la maquettes
maj du planning
ajout des disponibilités et affichage sur le profil
</commit_message>
<xml_diff>
--- a/planning.xlsx
+++ b/planning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
   <si>
     <t>Planning réel du TPI</t>
   </si>
@@ -85,6 +85,15 @@
   </si>
   <si>
     <t>Créer le fichier phptohtml</t>
+  </si>
+  <si>
+    <t>Continuer le profil</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>Disponibilités</t>
   </si>
 </sst>
 </file>
@@ -428,10 +437,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U23"/>
+  <dimension ref="A1:U26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,7 +670,7 @@
         <v>4.5138888888888888E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -668,7 +678,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -676,7 +686,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -684,7 +694,7 @@
         <v>1.3888888888888888E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -692,7 +702,7 @@
         <v>1.3888888888888888E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -700,7 +710,7 @@
         <v>6.9444444444444441E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -709,12 +719,33 @@
         <v>7.6388888888888895E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
       <c r="E23" s="2">
         <v>2.0833333333333332E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="F25" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
J'ai fait les pages de modification
J'ai modifier la manière d'afficher les  disponibilités
</commit_message>
<xml_diff>
--- a/planning.xlsx
+++ b/planning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
   <si>
     <t>Planning réel du TPI</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t>Disponibilités</t>
+  </si>
+  <si>
+    <t>Faire les pages de modification</t>
+  </si>
+  <si>
+    <t>Modifier les tableau des disponibilités</t>
   </si>
 </sst>
 </file>
@@ -437,11 +443,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U26"/>
+  <dimension ref="A1:U28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F26" sqref="F26"/>
+      <selection pane="topRight" activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -670,7 +676,7 @@
         <v>4.5138888888888888E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -678,7 +684,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -686,7 +692,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -694,7 +700,7 @@
         <v>1.3888888888888888E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -702,7 +708,7 @@
         <v>1.3888888888888888E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -710,7 +716,7 @@
         <v>6.9444444444444441E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -719,7 +725,7 @@
         <v>7.6388888888888895E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -727,7 +733,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -735,7 +741,7 @@
         <v>1.3888888888888888E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -743,9 +749,28 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
+      </c>
+      <c r="F26" s="2">
+        <v>5.9027777777777783E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G27" s="2">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="G28" s="2">
+        <v>2.7777777777777776E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
avancé sur les disponibilités
</commit_message>
<xml_diff>
--- a/planning.xlsx
+++ b/planning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
   <si>
     <t>Planning réel du TPI</t>
   </si>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>Modifier les tableau des disponibilités</t>
+  </si>
+  <si>
+    <t>modifierdisponibilites</t>
+  </si>
+  <si>
+    <t>Commentaires</t>
   </si>
 </sst>
 </file>
@@ -443,11 +449,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U28"/>
+  <dimension ref="A1:U30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H29" sqref="H29"/>
+      <selection pane="topRight" activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,7 +682,7 @@
         <v>4.5138888888888888E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -684,7 +690,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -692,7 +698,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -700,7 +706,7 @@
         <v>1.3888888888888888E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -708,7 +714,7 @@
         <v>1.3888888888888888E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -716,7 +722,7 @@
         <v>6.9444444444444441E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -725,7 +731,7 @@
         <v>7.6388888888888895E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -733,7 +739,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -741,15 +747,21 @@
         <v>1.3888888888888888E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
       <c r="F25" s="2">
         <v>8.3333333333333329E-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="I25" s="2">
+        <v>2.7777777777777776E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -757,7 +769,7 @@
         <v>5.9027777777777783E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -765,12 +777,31 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
       <c r="G28" s="2">
         <v>2.7777777777777776E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="H29" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="I29" s="2">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="H30" s="2">
+        <v>3.125E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
J'ai fait la recherche et afficher les résultats de la recherche j'ai modifier le nav et documenter toutes les fonctions de dao
</commit_message>
<xml_diff>
--- a/planning.xlsx
+++ b/planning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
   <si>
     <t>Planning réel du TPI</t>
   </si>
@@ -106,6 +106,15 @@
   </si>
   <si>
     <t>Commentaires</t>
+  </si>
+  <si>
+    <t>Faire la page rechercher</t>
+  </si>
+  <si>
+    <t>Créer la vue dans la BD</t>
+  </si>
+  <si>
+    <t>Fonction et page rechercher</t>
   </si>
 </sst>
 </file>
@@ -449,11 +458,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U30"/>
+  <dimension ref="A1:U33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I25" sqref="I25"/>
+      <selection pane="topRight" activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -682,7 +691,7 @@
         <v>4.5138888888888888E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -690,7 +699,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -698,7 +707,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -706,7 +715,7 @@
         <v>1.3888888888888888E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -714,7 +723,7 @@
         <v>1.3888888888888888E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -722,7 +731,7 @@
         <v>6.9444444444444441E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -731,7 +740,7 @@
         <v>7.6388888888888895E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -739,7 +748,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -747,7 +756,7 @@
         <v>1.3888888888888888E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -760,8 +769,26 @@
       <c r="I25" s="2">
         <v>2.7777777777777776E-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J25" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="K25" s="2">
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="L25" s="2">
+        <v>9.375E-2</v>
+      </c>
+      <c r="M25" s="2">
+        <v>0.15277777777777776</v>
+      </c>
+      <c r="N25" s="2">
+        <v>0.15625</v>
+      </c>
+      <c r="O25" s="2">
+        <v>6.9444444444444434E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -769,7 +796,7 @@
         <v>5.9027777777777783E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -777,7 +804,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -785,7 +812,7 @@
         <v>2.7777777777777776E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -796,12 +823,46 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
       <c r="H30" s="2">
         <v>3.125E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+      <c r="J31" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+      <c r="J32" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="K32" s="2"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+      <c r="J33" s="2">
+        <v>7.2916666666666671E-2</v>
+      </c>
+      <c r="K33" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="L33" s="2">
+        <v>6.25E-2</v>
+      </c>
+      <c r="O33" s="2">
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modifier l'affichage des dates
Ajouter l'affichage des espèce qu'on est d'accord de garder
</commit_message>
<xml_diff>
--- a/planning.xlsx
+++ b/planning.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
   <si>
     <t>Planning réel du TPI</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>Fonction et page rechercher</t>
+  </si>
+  <si>
+    <t>Changer l'affichage des dates</t>
   </si>
 </sst>
 </file>
@@ -458,11 +461,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U33"/>
+  <dimension ref="A1:U34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O26" sqref="O26"/>
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -691,7 +694,7 @@
         <v>4.5138888888888888E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -699,7 +702,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -707,7 +710,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -715,7 +718,7 @@
         <v>1.3888888888888888E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -723,7 +726,7 @@
         <v>1.3888888888888888E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -731,7 +734,7 @@
         <v>6.9444444444444441E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -740,7 +743,7 @@
         <v>7.6388888888888895E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -748,15 +751,18 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
       <c r="F24" s="2">
         <v>1.3888888888888888E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P24" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -788,7 +794,7 @@
         <v>6.9444444444444434E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -796,7 +802,7 @@
         <v>5.9027777777777783E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -804,7 +810,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -812,7 +818,7 @@
         <v>2.7777777777777776E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -823,7 +829,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -831,7 +837,7 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -839,7 +845,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -848,7 +854,7 @@
       </c>
       <c r="K32" s="2"/>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -863,6 +869,14 @@
       </c>
       <c r="O33" s="2">
         <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+      <c r="P34" s="2">
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
De petite modification renomage fonctions
</commit_message>
<xml_diff>
--- a/planning.xlsx
+++ b/planning.xlsx
@@ -465,7 +465,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P25" sqref="P25"/>
+      <selection pane="topRight" activeCell="Q28" sqref="Q28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,7 +694,7 @@
         <v>4.5138888888888888E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -702,7 +702,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -710,7 +710,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -718,7 +718,7 @@
         <v>1.3888888888888888E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -726,7 +726,7 @@
         <v>1.3888888888888888E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -734,7 +734,7 @@
         <v>6.9444444444444441E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -743,7 +743,7 @@
         <v>7.6388888888888895E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -751,7 +751,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -762,7 +762,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -793,8 +793,14 @@
       <c r="O25" s="2">
         <v>6.9444444444444434E-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P25" s="2">
+        <v>0.11458333333333333</v>
+      </c>
+      <c r="Q25" s="2">
+        <v>0.15277777777777776</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -802,7 +808,7 @@
         <v>5.9027777777777783E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -810,7 +816,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -818,7 +824,7 @@
         <v>2.7777777777777776E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -829,7 +835,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -837,7 +843,7 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -845,7 +851,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
Ajouter le manuel utilisateur
Modifier le nav de toutes les pages pour avoir l'onglet actif
</commit_message>
<xml_diff>
--- a/planning.xlsx
+++ b/planning.xlsx
@@ -465,7 +465,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q28" sqref="Q28"/>
+      <selection pane="topRight" activeCell="S26" sqref="S26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,7 +694,7 @@
         <v>4.5138888888888888E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -702,7 +702,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -710,7 +710,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -718,7 +718,7 @@
         <v>1.3888888888888888E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -726,7 +726,7 @@
         <v>1.3888888888888888E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -734,7 +734,7 @@
         <v>6.9444444444444441E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -743,7 +743,7 @@
         <v>7.6388888888888895E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -751,7 +751,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -762,7 +762,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -799,8 +799,14 @@
       <c r="Q25" s="2">
         <v>0.15277777777777776</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R25" s="2">
+        <v>0.15625</v>
+      </c>
+      <c r="S25" s="2">
+        <v>0.15277777777777776</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -808,7 +814,7 @@
         <v>5.9027777777777783E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -816,7 +822,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -824,7 +830,7 @@
         <v>2.7777777777777776E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -835,7 +841,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -843,7 +849,7 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -851,7 +857,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>

</xml_diff>